<commit_message>
kamal as a new employee
</commit_message>
<xml_diff>
--- a/Demo Project/TestFile.xlsx
+++ b/Demo Project/TestFile.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
   <si>
     <t>Employee ID</t>
   </si>
@@ -34,6 +34,12 @@
   </si>
   <si>
     <t>salam@gmail.com</t>
+  </si>
+  <si>
+    <t>kamal</t>
+  </si>
+  <si>
+    <t>kamal@gmail.com</t>
   </si>
 </sst>
 </file>
@@ -362,15 +368,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C2"/>
+  <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="15" customWidth="1"/>
+    <col min="3" max="3" width="22.42578125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
@@ -395,9 +402,21 @@
         <v>4</v>
       </c>
     </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>102</v>
+      </c>
+      <c r="B3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="C2" r:id="rId1"/>
+    <hyperlink ref="C3" r:id="rId2"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
jamal as a new record
</commit_message>
<xml_diff>
--- a/Demo Project/TestFile.xlsx
+++ b/Demo Project/TestFile.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
   <si>
     <t>Employee ID</t>
   </si>
@@ -40,6 +40,12 @@
   </si>
   <si>
     <t>kamal@gmail.com</t>
+  </si>
+  <si>
+    <t>Jamal</t>
+  </si>
+  <si>
+    <t>jamal@gmail.com</t>
   </si>
 </sst>
 </file>
@@ -368,10 +374,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C3"/>
+  <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -413,10 +419,22 @@
         <v>6</v>
       </c>
     </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>103</v>
+      </c>
+      <c r="B4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="C2" r:id="rId1"/>
     <hyperlink ref="C3" r:id="rId2"/>
+    <hyperlink ref="C4" r:id="rId3"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>